<commit_message>
GOAL 1 OF 3 ACCOMPLISHED :WORKTRAY GENERATION FINISHED! (state 1)!
</commit_message>
<xml_diff>
--- a/input/_worktray_template.xlsx
+++ b/input/_worktray_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afd218a83dc0962e/Documentos/Projects/santi-i001/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="11_F25DC773A252ABDACC10483D71DD50205ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55E4A9B3-4C91-412C-A4AC-82F454473D8D}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="11_F25DC773A252ABDACC10483D71DD50205ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D807314-D15C-4D3B-932A-CEA684BB8FCE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="base" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">base!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">base!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,6 +27,61 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Santiago G.</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6AA339F9-8966-478B-BA80-4742F20A3DC0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Santiago G.:
+Needs to be filled by S.C</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{A641D0B8-EA88-47BD-A319-2FB4E3081AD4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Santiago G.:
+Needs to be filled by S.C.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{2CB61327-CFDE-47DC-B856-85C3D621ED9E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Santiago G.:
+Needs to be filled by S.C</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
@@ -64,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,11 +132,14 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,8 +152,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,24 +167,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -143,6 +246,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -193,6 +306,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -230,63 +353,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF2C2454"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -308,25 +374,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D172F1F7-D454-4826-8FED-1EF62A112B63}" name="WORKTRAY" displayName="WORKTRAY" ref="A1:J2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:J2" xr:uid="{D172F1F7-D454-4826-8FED-1EF62A112B63}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{DDC164F9-268D-49EC-B2DD-23C2FADAE8F5}" name="project_id"/>
-    <tableColumn id="10" xr3:uid="{DA08E658-81EA-4CD0-91B1-CC24AA9A5A53}" name="project_finished"/>
-    <tableColumn id="2" xr3:uid="{237DE627-DDBD-42C4-AECE-B32189F0F45D}" name="planning_file_path" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{0C8C564F-7B76-4C37-A591-C4593AEFD0B0}" name="clickup_data_extracted" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{489FA108-8A10-4430-9996-EB21FC4F8DC1}" name="clickup_data_path" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{4FFD417E-381E-4534-A172-B285BEF21F7D}" name="raw_file_path" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{63D4FB86-5CBC-4453-A254-0A1D2F65BBCD}" name="processed_file_path" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{AD9B35FA-8899-452A-BDE0-1DC7EE1E03D5}" name="planning_file_updated" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{F66BA3D3-8C50-4CAD-8926-FBA4ABF0FCAE}" name="execution_datetime" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{BAE5FA06-B904-4B48-AB67-8B59172157B9}" name="observations"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,89 +638,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="112.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="123.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D2"/>
-      <c r="E2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="L2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L4"/>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576 D1:D1048576 H1:H1048576">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+  <autoFilter ref="A1:J1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H1048576">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 D2 H2" xr:uid="{A39D10A8-E531-42C9-80AA-034CBBCB849E}">
-      <formula1>"FALSE,TRUE"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <conditionalFormatting sqref="E1">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHECKPOINT: JSON PROCESSING AT 50%
</commit_message>
<xml_diff>
--- a/input/_worktray_template.xlsx
+++ b/input/_worktray_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afd218a83dc0962e/Documentos/Projects/santi-i001/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="11_F25DC773A252ABDACC10483D71DD50205ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D807314-D15C-4D3B-932A-CEA684BB8FCE}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC10483D71DD50205ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20281461-43C6-4C02-BD50-2442A9BB894D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,22 @@
     <author>Santiago G.</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6AA339F9-8966-478B-BA80-4742F20A3DC0}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7768E1A9-B110-4C6A-850B-BA636B383244}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Santiago G.:
+Must be filled by SC with the Customer folder name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2B9752BF-2846-4267-94AE-F57FE4432ED4}">
       <text>
         <r>
           <rPr>
@@ -48,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{A641D0B8-EA88-47BD-A319-2FB4E3081AD4}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{F67A84D8-312B-4A5F-B564-A661621E8905}">
       <text>
         <r>
           <rPr>
@@ -63,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{2CB61327-CFDE-47DC-B856-85C3D621ED9E}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{190318F9-6059-43FA-9B45-95C9FD685447}">
       <text>
         <r>
           <rPr>
@@ -83,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>project_id</t>
   </si>
@@ -113,6 +128,9 @@
   </si>
   <si>
     <t>processed_file_path</t>
+  </si>
+  <si>
+    <t>customer</t>
   </si>
 </sst>
 </file>
@@ -130,12 +148,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -200,120 +218,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -656,8 +574,8 @@
     <col min="6" max="6" width="112.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="123.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -665,33 +583,36 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -707,52 +628,20 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
+  <conditionalFormatting sqref="A2:XFD1048576 L1:XFD1">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E2)))</formula>
+  <conditionalFormatting sqref="A1:K1">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F1)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>